<commit_message>
Ghost Inventory Class added and fixed. Also added new inset statement
</commit_message>
<xml_diff>
--- a/Replenishment/support document/Store List.xlsx
+++ b/Replenishment/support document/Store List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\OneDrive\WinWin Staff Folders\Michael\Replenishment program\Replenishment\support document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDA9ABC-0EB7-45A2-8784-92571C493BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6999870-A9C8-47FA-BAB0-6D6DFC344158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{81352D18-0B16-43AE-9382-0D99017645F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81352D18-0B16-43AE-9382-0D99017645F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>store_type_input</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Follett Price</t>
+  </si>
+  <si>
+    <t>Store Notes Suffix</t>
   </si>
 </sst>
 </file>
@@ -604,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C8F5AE-76EF-4A0C-9E95-B0978FB28F19}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,9 +618,10 @@
     <col min="1" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,8 +634,11 @@
       <c r="D1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -645,7 +652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -659,7 +666,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -673,7 +680,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -687,7 +694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -701,7 +708,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -715,7 +722,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -729,7 +736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -743,7 +750,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -757,7 +764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -771,7 +778,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -785,7 +792,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -799,7 +806,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -813,7 +820,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -827,7 +834,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>

</xml_diff>